<commit_message>
Update awardees, blog, auth, and add new initiatives pages
</commit_message>
<xml_diff>
--- a/public/top100 Africa future Leaders 2025.xlsx
+++ b/public/top100 Africa future Leaders 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\top100\v0_Top100Afl - Copy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0976A525-217B-4162-B831-C7BFC25233EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D2CCA5-F340-4733-ACB7-BE97932A3A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="3000" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -6331,8 +6331,8 @@
   <dimension ref="A1:J419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>